<commit_message>
updated logic for extracting basic model data
</commit_message>
<xml_diff>
--- a/example metadata settings files/weh column list.xlsx
+++ b/example metadata settings files/weh column list.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wardc\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\VevoLab_Data_Extraction_Helper\example metadata settings files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD1CB9E8-E646-46E2-B939-3A21F9A8364B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B90743F8-C93B-42B3-A186-4E9CB7FD6BE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-9870" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{B694D1C7-74D3-4338-806C-289403162B5E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{B694D1C7-74D3-4338-806C-289403162B5E}"/>
   </bookViews>
   <sheets>
-    <sheet name="ColumnNames" sheetId="5" r:id="rId1"/>
-    <sheet name="DerivedData" sheetId="6" r:id="rId2"/>
+    <sheet name="column names" sheetId="5" r:id="rId1"/>
+    <sheet name="derived data" sheetId="6" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>

</xml_diff>